<commit_message>
Se empieza a ajustar el menu segun administrador
</commit_message>
<xml_diff>
--- a/backend/ORGANIZACION DE MENUS Y MODULOS.xlsx
+++ b/backend/ORGANIZACION DE MENUS Y MODULOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\FP\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A38837D-50A8-4063-98CB-1C2D51FB9D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B095318D-531D-4231-BDEA-47FC788253D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F3A673B7-C585-49DB-9A40-1BDF61776621}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="25">
   <si>
     <t>Administrador</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t xml:space="preserve">Usuario </t>
+  </si>
+  <si>
+    <t>8. Cerrar sesion</t>
   </si>
 </sst>
 </file>
@@ -121,7 +124,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -149,6 +152,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -188,19 +197,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -517,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845D673F-1DCD-49C3-8B84-2BE5A8585294}">
-  <dimension ref="B2:K24"/>
+  <dimension ref="B2:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14:K20"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,296 +543,310 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="3"/>
-      <c r="J2" s="4" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="1"/>
+      <c r="J2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="4"/>
+      <c r="K2" s="6"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="4"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="5"/>
-      <c r="H3" s="3"/>
-      <c r="J3" s="6" t="s">
+      <c r="H3" s="1"/>
+      <c r="J3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="6"/>
+      <c r="K3" s="3"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="4"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G4" s="5"/>
-      <c r="H4" s="3"/>
-      <c r="J4" s="6" t="s">
+      <c r="H4" s="1"/>
+      <c r="J4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="6"/>
+      <c r="K4" s="3"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="4"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="5"/>
-      <c r="H5" s="3"/>
-      <c r="J5" s="6" t="s">
+      <c r="H5" s="1"/>
+      <c r="J5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="6"/>
+      <c r="K5" s="3"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="5"/>
-      <c r="H6" s="3"/>
-      <c r="J6" s="6" t="s">
+      <c r="H6" s="1"/>
+      <c r="J6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="6"/>
+      <c r="K6" s="3"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="5" t="s">
         <v>15</v>
       </c>
       <c r="G7" s="5"/>
-      <c r="H7" s="3"/>
-      <c r="J7" s="6" t="s">
+      <c r="H7" s="1"/>
+      <c r="J7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="6"/>
+      <c r="K7" s="3"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="4"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="6"/>
+      <c r="K8" s="3"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="4"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1" t="s">
+      <c r="C13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="F13" s="7" t="s">
+      <c r="C14" s="4"/>
+      <c r="F14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="J13" s="7" t="s">
+      <c r="G14" s="7"/>
+      <c r="J14" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="K13" s="7"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
+      <c r="K14" s="7"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="F14" s="5" t="s">
+      <c r="C15" s="4"/>
+      <c r="F15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="5"/>
-      <c r="J14" s="5" t="s">
+      <c r="G15" s="5"/>
+      <c r="J15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="F15" s="5" t="s">
+      <c r="C16" s="4"/>
+      <c r="F16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="5"/>
-      <c r="J15" s="6" t="s">
+      <c r="G16" s="5"/>
+      <c r="J16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="F16" s="5" t="s">
+      <c r="C17" s="4"/>
+      <c r="F17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="5"/>
-      <c r="J16" s="6" t="s">
+      <c r="G17" s="5"/>
+      <c r="J17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K16" s="6"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="F17" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="5"/>
-      <c r="J17" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K17" s="6"/>
+      <c r="K17" s="3"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18" s="7"/>
       <c r="F18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="J18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="F19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="5"/>
-      <c r="J18" s="6" t="s">
+      <c r="G19" s="5"/>
+      <c r="J19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K18" s="6"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="7" t="s">
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="J19" s="6" t="s">
+      <c r="C20" s="4"/>
+      <c r="F20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="J20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K19" s="6"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="5"/>
-      <c r="J20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K20" s="6"/>
+      <c r="K20" s="3"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21" s="5"/>
+      <c r="J21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" s="3"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22" s="5"/>
+      <c r="J22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K22" s="4"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23" s="5"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="5"/>
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="47">
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
+  <mergeCells count="51">
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="J3:K3"/>
@@ -831,20 +854,32 @@
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="J7:K7"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Quedo listo la primera funcion de la parte del administrador
</commit_message>
<xml_diff>
--- a/backend/ORGANIZACION DE MENUS Y MODULOS.xlsx
+++ b/backend/ORGANIZACION DE MENUS Y MODULOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\FP\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B095318D-531D-4231-BDEA-47FC788253D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B596C90B-EC33-4674-A8EF-1C56FA4D949A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F3A673B7-C585-49DB-9A40-1BDF61776621}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="26">
   <si>
     <t>Administrador</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>8. Cerrar sesion</t>
+  </si>
+  <si>
+    <t>Funciones ya hechas según el  Administrador</t>
   </si>
 </sst>
 </file>
@@ -197,9 +200,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -207,6 +207,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -526,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845D673F-1DCD-49C3-8B84-2BE5A8585294}">
-  <dimension ref="B2:K26"/>
+  <dimension ref="B2:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,137 +545,144 @@
     <col min="11" max="11" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="5"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="6"/>
+      <c r="G2" s="5"/>
       <c r="H2" s="1"/>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="6"/>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="K2" s="5"/>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="3"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="4"/>
       <c r="H3" s="1"/>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+      <c r="K3" s="6"/>
+      <c r="M3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="G4" s="4"/>
       <c r="H4" s="1"/>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="3"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="5"/>
+      <c r="G5" s="4"/>
       <c r="H5" s="1"/>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="3"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+      <c r="K5" s="6"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="3"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="G6" s="4"/>
       <c r="H6" s="1"/>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="3"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="3"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="5"/>
+      <c r="G7" s="4"/>
       <c r="H7" s="1"/>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="3"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="3"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="K8" s="6"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>0</v>
       </c>
@@ -685,11 +695,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="3"/>
       <c r="F14" s="7" t="s">
         <v>6</v>
       </c>
@@ -699,142 +709,160 @@
       </c>
       <c r="K14" s="7"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="F15" s="5" t="s">
+      <c r="C15" s="3"/>
+      <c r="F15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="5"/>
-      <c r="J15" s="5" t="s">
+      <c r="G15" s="4"/>
+      <c r="J15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K15" s="5"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="F16" s="5" t="s">
+      <c r="C16" s="3"/>
+      <c r="F16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="5"/>
-      <c r="J16" s="3" t="s">
+      <c r="G16" s="4"/>
+      <c r="J16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="K16" s="3"/>
+      <c r="K16" s="6"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="F17" s="5" t="s">
+      <c r="C17" s="3"/>
+      <c r="F17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="5"/>
-      <c r="J17" s="3" t="s">
+      <c r="G17" s="4"/>
+      <c r="J17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="K17" s="3"/>
+      <c r="K17" s="6"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C18" s="7"/>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="5"/>
-      <c r="J18" s="3" t="s">
+      <c r="G18" s="4"/>
+      <c r="J18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="K18" s="3"/>
+      <c r="K18" s="6"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="F19" s="5" t="s">
+      <c r="C19" s="3"/>
+      <c r="F19" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="5"/>
-      <c r="J19" s="3" t="s">
+      <c r="G19" s="4"/>
+      <c r="J19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K19" s="3"/>
+      <c r="K19" s="6"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="F20" s="4" t="s">
+      <c r="C20" s="3"/>
+      <c r="F20" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="4"/>
-      <c r="J20" s="3" t="s">
+      <c r="G20" s="3"/>
+      <c r="J20" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K20" s="3"/>
+      <c r="K20" s="6"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="J21" s="3" t="s">
+      <c r="C21" s="4"/>
+      <c r="J21" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K21" s="3"/>
+      <c r="K21" s="6"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="J22" s="4" t="s">
+      <c r="C22" s="4"/>
+      <c r="J22" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K22" s="4"/>
+      <c r="K22" s="3"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="5"/>
+      <c r="C23" s="4"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="5"/>
+      <c r="C24" s="4"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="5"/>
+      <c r="C25" s="4"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="4"/>
+      <c r="C26" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="51">
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="F20:G20"/>
+  <mergeCells count="52">
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -847,39 +875,22 @@
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F6:G6"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="F20:G20"/>
     <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="J21:K21"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Quedo lista las funciones de usuarios para el administrador faltan las demas
</commit_message>
<xml_diff>
--- a/backend/ORGANIZACION DE MENUS Y MODULOS.xlsx
+++ b/backend/ORGANIZACION DE MENUS Y MODULOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\FP\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B596C90B-EC33-4674-A8EF-1C56FA4D949A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8264862-30A8-4E72-84B2-E5721C07494C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F3A673B7-C585-49DB-9A40-1BDF61776621}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="26">
   <si>
     <t>Administrador</t>
   </si>
@@ -54,15 +54,6 @@
     <t>4. Buscar Usuario por telefono</t>
   </si>
   <si>
-    <t>5. Login de usuario</t>
-  </si>
-  <si>
-    <t>6. Actualizar usuario</t>
-  </si>
-  <si>
-    <t>7. Eliminar Usuario</t>
-  </si>
-  <si>
     <t>MODULO PRODUCTOS</t>
   </si>
   <si>
@@ -108,10 +99,19 @@
     <t xml:space="preserve">Usuario </t>
   </si>
   <si>
-    <t>8. Cerrar sesion</t>
-  </si>
-  <si>
     <t>Funciones ya hechas según el  Administrador</t>
+  </si>
+  <si>
+    <t>0. Login de usuario</t>
+  </si>
+  <si>
+    <t>5. Actualizar usuario</t>
+  </si>
+  <si>
+    <t>6. Eliminar Usuario</t>
+  </si>
+  <si>
+    <t>7. Cerrar sesion</t>
   </si>
 </sst>
 </file>
@@ -200,19 +200,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -532,7 +532,7 @@
   <dimension ref="B2:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,142 +543,163 @@
     <col min="7" max="7" width="22" customWidth="1"/>
     <col min="8" max="9" width="10" customWidth="1"/>
     <col min="11" max="11" width="24" customWidth="1"/>
+    <col min="14" max="14" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="7"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="5"/>
+      <c r="F2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="7"/>
       <c r="H2" s="1"/>
-      <c r="J2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="5"/>
+      <c r="J2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="7"/>
       <c r="M2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="4"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="4"/>
+      <c r="F3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="3"/>
       <c r="H3" s="1"/>
-      <c r="J3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" s="6"/>
-      <c r="M3" s="3" t="s">
+      <c r="J3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="M3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="3"/>
+      <c r="N3" s="4"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="4"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="4"/>
+      <c r="F4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="3"/>
       <c r="H4" s="1"/>
-      <c r="J4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="6"/>
+      <c r="J4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="M4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" s="4"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="4"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="4"/>
+      <c r="F5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="3"/>
       <c r="H5" s="1"/>
-      <c r="J5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="6"/>
+      <c r="J5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="5"/>
+      <c r="M5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="N5" s="4"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="4"/>
+      <c r="F6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="3"/>
       <c r="H6" s="1"/>
-      <c r="J6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" s="6"/>
+      <c r="J6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="5"/>
+      <c r="M6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N6" s="4"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="3"/>
+      <c r="B7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="4"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="4"/>
+      <c r="F7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="3"/>
       <c r="H7" s="1"/>
-      <c r="J7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7" s="6"/>
+      <c r="J7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="5"/>
+      <c r="M7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N7" s="4"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="3"/>
+      <c r="B8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="4"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="J8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K8" s="6"/>
+      <c r="J8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="5"/>
+      <c r="M8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N8" s="4"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="3"/>
+      <c r="B9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="4"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="3"/>
+      <c r="B10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="4"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
@@ -689,192 +710,159 @@
       <c r="C13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="F14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="G14" s="6"/>
+      <c r="J14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="6"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="F15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="J15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="F16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="J16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="F17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="J17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="F18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="J18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="F14" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="7"/>
-      <c r="J14" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="K14" s="7"/>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="F15" s="4" t="s">
+      <c r="C19" s="4"/>
+      <c r="F19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="J19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="F20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="J20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="J21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K21" s="5"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="J22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K22" s="4"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="4"/>
-      <c r="J15" s="4" t="s">
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K15" s="4"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="F16" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="4"/>
-      <c r="J16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K16" s="6"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="F17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="4"/>
-      <c r="J17" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K17" s="6"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="F18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="4"/>
-      <c r="J18" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K18" s="6"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="F19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="4"/>
-      <c r="J19" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K19" s="6"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="F20" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G20" s="3"/>
-      <c r="J20" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K20" s="6"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="J21" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="K21" s="6"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="J22" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K22" s="3"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="4"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="4"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="4"/>
+      <c r="C25" s="3"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="3"/>
+      <c r="B26" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="52">
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
+  <mergeCells count="57">
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M8:N8"/>
     <mergeCell ref="J22:K22"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
@@ -891,6 +879,44 @@
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Se adelanto hasta la funcio 8 del menu de adminsitrador (la funcion 8 esta de ceros)
</commit_message>
<xml_diff>
--- a/backend/ORGANIZACION DE MENUS Y MODULOS.xlsx
+++ b/backend/ORGANIZACION DE MENUS Y MODULOS.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\FP\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8264862-30A8-4E72-84B2-E5721C07494C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84AEB86-B944-45E2-8E08-794BFADC86F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F3A673B7-C585-49DB-9A40-1BDF61776621}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="29">
   <si>
     <t>Administrador</t>
   </si>
@@ -112,6 +113,15 @@
   </si>
   <si>
     <t>7. Cerrar sesion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To do list </t>
+  </si>
+  <si>
+    <t>1. Que quede bien los menus con cada funcion dependiendo del usuario</t>
+  </si>
+  <si>
+    <t>2. Mirar las validaciones por cada usuario (admin, ven usu)</t>
   </si>
 </sst>
 </file>
@@ -127,7 +137,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,6 +174,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -192,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -200,21 +216,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,7 +549,7 @@
   <dimension ref="B2:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,159 +564,163 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="7"/>
+      <c r="G2" s="6"/>
       <c r="H2" s="1"/>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="7"/>
+      <c r="K2" s="6"/>
       <c r="M2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="3"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="G3" s="5"/>
       <c r="H3" s="1"/>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="5"/>
-      <c r="M3" s="4" t="s">
+      <c r="K3" s="4"/>
+      <c r="M3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="4"/>
+      <c r="N3" s="3"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="5"/>
       <c r="H4" s="1"/>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="5"/>
-      <c r="M4" s="4" t="s">
+      <c r="K4" s="4"/>
+      <c r="M4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="N4" s="4"/>
+      <c r="N4" s="3"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="3"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="3"/>
+      <c r="G5" s="5"/>
       <c r="H5" s="1"/>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="5"/>
-      <c r="M5" s="4" t="s">
+      <c r="K5" s="4"/>
+      <c r="M5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N5" s="4"/>
+      <c r="N5" s="3"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="3"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="5"/>
       <c r="H6" s="1"/>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="5"/>
-      <c r="M6" s="4" t="s">
+      <c r="K6" s="4"/>
+      <c r="M6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="4"/>
+      <c r="N6" s="3"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="3"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="3"/>
+      <c r="G7" s="5"/>
       <c r="H7" s="1"/>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="5"/>
-      <c r="M7" s="4" t="s">
+      <c r="K7" s="4"/>
+      <c r="M7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="N7" s="4"/>
+      <c r="N7" s="3"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="3"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="5"/>
-      <c r="M8" s="4" t="s">
+      <c r="K8" s="4"/>
+      <c r="M8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="N8" s="4"/>
+      <c r="N8" s="3"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
+      <c r="M9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N9" s="5"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
@@ -717,192 +738,149 @@
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="F14" s="6" t="s">
+      <c r="C14" s="3"/>
+      <c r="F14" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="J14" s="6" t="s">
+      <c r="G14" s="7"/>
+      <c r="J14" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K14" s="6"/>
+      <c r="K14" s="7"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="F15" s="3" t="s">
+      <c r="C15" s="3"/>
+      <c r="F15" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="3"/>
-      <c r="J15" s="3" t="s">
+      <c r="G15" s="5"/>
+      <c r="J15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K15" s="3"/>
+      <c r="K15" s="5"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="F16" s="3" t="s">
+      <c r="C16" s="3"/>
+      <c r="F16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="3"/>
-      <c r="J16" s="5" t="s">
+      <c r="G16" s="5"/>
+      <c r="J16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K16" s="5"/>
+      <c r="K16" s="4"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="F17" s="3" t="s">
+      <c r="C17" s="3"/>
+      <c r="F17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="3"/>
-      <c r="J17" s="5" t="s">
+      <c r="G17" s="5"/>
+      <c r="J17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K17" s="5"/>
+      <c r="K17" s="4"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="F18" s="3" t="s">
+      <c r="C18" s="7"/>
+      <c r="F18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="3"/>
-      <c r="J18" s="5" t="s">
+      <c r="G18" s="5"/>
+      <c r="J18" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K18" s="5"/>
+      <c r="K18" s="4"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="F19" s="3" t="s">
+      <c r="C19" s="3"/>
+      <c r="F19" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="3"/>
-      <c r="J19" s="5" t="s">
+      <c r="G19" s="5"/>
+      <c r="J19" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="K19" s="5"/>
+      <c r="K19" s="4"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="F20" s="4" t="s">
+      <c r="C20" s="3"/>
+      <c r="F20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="4"/>
-      <c r="J20" s="5" t="s">
+      <c r="G20" s="3"/>
+      <c r="J20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K20" s="5"/>
+      <c r="K20" s="4"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="J21" s="5" t="s">
+      <c r="C21" s="5"/>
+      <c r="J21" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K21" s="5"/>
+      <c r="K21" s="4"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="J22" s="4" t="s">
+      <c r="C22" s="5"/>
+      <c r="J22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K22" s="4"/>
+      <c r="K22" s="3"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="3"/>
+      <c r="C23" s="5"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="3"/>
+      <c r="C24" s="5"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="3"/>
+      <c r="C25" s="5"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="4"/>
+      <c r="C26" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="57">
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
+  <mergeCells count="58">
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="B19:C19"/>
@@ -917,8 +895,85 @@
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7BE8726-823E-41B9-BEEC-4BD805B69C0C}">
+  <dimension ref="B2:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="64.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se adelentaron las funciones de los administradores faltan los vendedores y usuario
</commit_message>
<xml_diff>
--- a/backend/ORGANIZACION DE MENUS Y MODULOS.xlsx
+++ b/backend/ORGANIZACION DE MENUS Y MODULOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\FP\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84AEB86-B944-45E2-8E08-794BFADC86F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6CB12D-6EF6-497E-9CC3-4DAE798085AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F3A673B7-C585-49DB-9A40-1BDF61776621}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="30">
   <si>
     <t>Administrador</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>2. Mirar las validaciones por cada usuario (admin, ven usu)</t>
+  </si>
+  <si>
+    <t>Funciones ya hechas según el  Vendedor</t>
   </si>
 </sst>
 </file>
@@ -216,10 +219,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -228,10 +235,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,165 +567,181 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="6"/>
+      <c r="G2" s="8"/>
       <c r="H2" s="1"/>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="6"/>
+      <c r="K2" s="8"/>
       <c r="M2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="4"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="7"/>
       <c r="H3" s="1"/>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="4"/>
-      <c r="M3" s="3" t="s">
+      <c r="K3" s="5"/>
+      <c r="M3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="3"/>
+      <c r="N3" s="4"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="4"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="G4" s="7"/>
       <c r="H4" s="1"/>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="4"/>
-      <c r="M4" s="3" t="s">
+      <c r="K4" s="5"/>
+      <c r="M4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N4" s="3"/>
+      <c r="N4" s="4"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="4"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="5"/>
+      <c r="G5" s="7"/>
       <c r="H5" s="1"/>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="4"/>
-      <c r="M5" s="3" t="s">
+      <c r="K5" s="5"/>
+      <c r="M5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="N5" s="3"/>
+      <c r="N5" s="4"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="G6" s="7"/>
       <c r="H6" s="1"/>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="4"/>
-      <c r="M6" s="3" t="s">
+      <c r="K6" s="5"/>
+      <c r="M6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="3"/>
+      <c r="N6" s="4"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="5"/>
+      <c r="G7" s="7"/>
       <c r="H7" s="1"/>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="4"/>
-      <c r="M7" s="3" t="s">
+      <c r="K7" s="5"/>
+      <c r="M7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N7" s="3"/>
+      <c r="N7" s="4"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="4"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="4"/>
-      <c r="M8" s="3" t="s">
+      <c r="K8" s="5"/>
+      <c r="M8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="N8" s="3"/>
+      <c r="N8" s="4"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="4"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="M9" s="5" t="s">
+      <c r="M9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="N9" s="5"/>
+      <c r="N9" s="7"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="4"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
+      <c r="M10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="N10" s="7"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="N11" s="7"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="N12" s="7"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
@@ -736,181 +755,173 @@
       <c r="J13" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="M13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N13" s="7"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="F14" s="7" t="s">
+      <c r="C14" s="4"/>
+      <c r="F14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="7"/>
-      <c r="J14" s="7" t="s">
+      <c r="G14" s="6"/>
+      <c r="J14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K14" s="7"/>
+      <c r="K14" s="6"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="F15" s="5" t="s">
+      <c r="C15" s="4"/>
+      <c r="F15" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="5"/>
-      <c r="J15" s="5" t="s">
+      <c r="G15" s="7"/>
+      <c r="J15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K15" s="5"/>
+      <c r="K15" s="7"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="F16" s="5" t="s">
+      <c r="C16" s="4"/>
+      <c r="F16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="5"/>
-      <c r="J16" s="4" t="s">
+      <c r="G16" s="7"/>
+      <c r="J16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K16" s="4"/>
+      <c r="K16" s="5"/>
+      <c r="M16" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="F17" s="5" t="s">
+      <c r="C17" s="4"/>
+      <c r="F17" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="5"/>
-      <c r="J17" s="4" t="s">
+      <c r="G17" s="7"/>
+      <c r="J17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K17" s="4"/>
+      <c r="K17" s="5"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="F18" s="5" t="s">
+      <c r="C18" s="6"/>
+      <c r="F18" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="5"/>
-      <c r="J18" s="4" t="s">
+      <c r="G18" s="7"/>
+      <c r="J18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K18" s="4"/>
+      <c r="K18" s="5"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="F19" s="5" t="s">
+      <c r="C19" s="4"/>
+      <c r="F19" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="5"/>
-      <c r="J19" s="4" t="s">
+      <c r="G19" s="7"/>
+      <c r="J19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K19" s="4"/>
+      <c r="K19" s="5"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="F20" s="3" t="s">
+      <c r="C20" s="4"/>
+      <c r="F20" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="3"/>
-      <c r="J20" s="4" t="s">
+      <c r="G20" s="4"/>
+      <c r="J20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K20" s="4"/>
+      <c r="K20" s="5"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="J21" s="4" t="s">
+      <c r="C21" s="7"/>
+      <c r="J21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K21" s="4"/>
+      <c r="K21" s="5"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="J22" s="3" t="s">
+      <c r="C22" s="7"/>
+      <c r="J22" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K22" s="3"/>
+      <c r="K22" s="4"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="5"/>
+      <c r="C23" s="7"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="5"/>
+      <c r="C24" s="7"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="5"/>
+      <c r="C25" s="7"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="3"/>
+      <c r="C26" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="58">
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
+  <mergeCells count="62">
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M13:N13"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="J8:K8"/>
@@ -927,18 +938,37 @@
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M9:N9"/>
     <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -964,7 +994,7 @@
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="3" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se adelentaron las funciones de los vendedores faltan usuarios
</commit_message>
<xml_diff>
--- a/backend/ORGANIZACION DE MENUS Y MODULOS.xlsx
+++ b/backend/ORGANIZACION DE MENUS Y MODULOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\FP\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6CB12D-6EF6-497E-9CC3-4DAE798085AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC435FE-59F7-4D2B-830C-AE9C289F6FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F3A673B7-C585-49DB-9A40-1BDF61776621}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="30">
   <si>
     <t>Administrador</t>
   </si>
@@ -223,13 +223,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -552,7 +552,7 @@
   <dimension ref="B2:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,15 +593,15 @@
       <c r="C3" s="4"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="7"/>
+      <c r="G3" s="6"/>
       <c r="H3" s="1"/>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="5"/>
+      <c r="K3" s="7"/>
       <c r="M3" s="4" t="s">
         <v>2</v>
       </c>
@@ -614,15 +614,15 @@
       <c r="C4" s="4"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="7"/>
+      <c r="G4" s="6"/>
       <c r="H4" s="1"/>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="5"/>
+      <c r="K4" s="7"/>
       <c r="M4" s="4" t="s">
         <v>3</v>
       </c>
@@ -635,15 +635,15 @@
       <c r="C5" s="4"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="7"/>
+      <c r="G5" s="6"/>
       <c r="H5" s="1"/>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="5"/>
+      <c r="K5" s="7"/>
       <c r="M5" s="4" t="s">
         <v>4</v>
       </c>
@@ -656,15 +656,15 @@
       <c r="C6" s="4"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="7"/>
+      <c r="G6" s="6"/>
       <c r="H6" s="1"/>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="5"/>
+      <c r="K6" s="7"/>
       <c r="M6" s="4" t="s">
         <v>5</v>
       </c>
@@ -677,15 +677,15 @@
       <c r="C7" s="4"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="7"/>
+      <c r="G7" s="6"/>
       <c r="H7" s="1"/>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="5"/>
+      <c r="K7" s="7"/>
       <c r="M7" s="4" t="s">
         <v>23</v>
       </c>
@@ -698,10 +698,10 @@
       <c r="C8" s="4"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="5"/>
+      <c r="K8" s="7"/>
       <c r="M8" s="4" t="s">
         <v>24</v>
       </c>
@@ -714,10 +714,10 @@
       <c r="C9" s="4"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="M9" s="7" t="s">
+      <c r="M9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N9" s="7"/>
+      <c r="N9" s="6"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
@@ -726,22 +726,22 @@
       <c r="C10" s="4"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="M10" s="7" t="s">
+      <c r="M10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="N10" s="7"/>
+      <c r="N10" s="6"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="M11" s="7" t="s">
+      <c r="M11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="N11" s="7"/>
+      <c r="N11" s="6"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="M12" s="7" t="s">
+      <c r="M12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="N12" s="7"/>
+      <c r="N12" s="6"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
@@ -755,99 +755,111 @@
       <c r="J13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M13" s="7" t="s">
+      <c r="M13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N13" s="7"/>
+      <c r="N13" s="6"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="J14" s="6" t="s">
+      <c r="G14" s="5"/>
+      <c r="J14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K14" s="6"/>
+      <c r="K14" s="5"/>
+      <c r="M14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N14" s="4"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="4"/>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="7"/>
-      <c r="J15" s="7" t="s">
+      <c r="G15" s="6"/>
+      <c r="J15" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K15" s="7"/>
+      <c r="K15" s="6"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C16" s="4"/>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="7"/>
-      <c r="J16" s="5" t="s">
+      <c r="G16" s="6"/>
+      <c r="J16" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="K16" s="5"/>
-      <c r="M16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K16" s="7"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="7"/>
-      <c r="J17" s="5" t="s">
+      <c r="G17" s="6"/>
+      <c r="J17" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="K17" s="5"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="6" t="s">
+      <c r="K17" s="7"/>
+      <c r="M17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="F18" s="7" t="s">
+      <c r="C18" s="5"/>
+      <c r="F18" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="7"/>
-      <c r="J18" s="5" t="s">
+      <c r="G18" s="6"/>
+      <c r="J18" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="K18" s="5"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="7"/>
+      <c r="M18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="N18" s="6"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="7"/>
-      <c r="J19" s="5" t="s">
+      <c r="G19" s="6"/>
+      <c r="J19" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K19" s="5"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="7"/>
+      <c r="M19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N19" s="6"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>24</v>
       </c>
@@ -856,72 +868,110 @@
         <v>25</v>
       </c>
       <c r="G20" s="4"/>
-      <c r="J20" s="5" t="s">
+      <c r="J20" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K20" s="5"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="7" t="s">
+      <c r="K20" s="7"/>
+      <c r="M20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N20" s="6"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="J21" s="5" t="s">
+      <c r="C21" s="6"/>
+      <c r="J21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K21" s="5"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="7" t="s">
+      <c r="K21" s="7"/>
+      <c r="M21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N21" s="6"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="7"/>
+      <c r="C22" s="6"/>
       <c r="J22" s="4" t="s">
         <v>25</v>
       </c>
       <c r="K22" s="4"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
+      <c r="M22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N22" s="6"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="7"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="7" t="s">
+      <c r="C23" s="6"/>
+      <c r="M23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N23" s="4"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="7"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="7" t="s">
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B25" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="7"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="62">
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M13:N13"/>
+  <mergeCells count="69">
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="J8:K8"/>
@@ -938,37 +988,22 @@
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M18:N18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>